<commit_message>
jan 13 2025 4:38 am
</commit_message>
<xml_diff>
--- a/clause_content_variety_latest_clauses.xlsx
+++ b/clause_content_variety_latest_clauses.xlsx
@@ -2872,7 +2872,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -2884,7 +2884,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -2896,7 +2896,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -2908,7 +2908,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -2920,7 +2920,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -2932,7 +2932,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -2944,7 +2944,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -2956,7 +2956,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -2968,7 +2968,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -2980,7 +2980,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -2992,7 +2992,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -3004,7 +3004,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -3016,7 +3016,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -3028,7 +3028,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -3040,7 +3040,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -3052,7 +3052,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -3064,7 +3064,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -3076,7 +3076,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -3088,7 +3088,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -3112,7 +3112,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -3124,7 +3124,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -3136,7 +3136,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -3148,7 +3148,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -3160,7 +3160,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -3172,7 +3172,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -3184,7 +3184,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -3196,7 +3196,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -3208,7 +3208,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -3220,7 +3220,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -3232,7 +3232,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -3244,7 +3244,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -3256,7 +3256,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -3280,7 +3280,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -3292,7 +3292,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -3304,7 +3304,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -3316,7 +3316,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -3328,7 +3328,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -3364,7 +3364,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -3376,7 +3376,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -3388,7 +3388,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -3400,7 +3400,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -3412,7 +3412,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -3424,7 +3424,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -3448,7 +3448,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -3460,7 +3460,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -3472,7 +3472,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -3484,7 +3484,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -3496,7 +3496,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -3508,7 +3508,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -3520,7 +3520,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -3532,7 +3532,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -3544,7 +3544,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -3556,7 +3556,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -3568,7 +3568,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -3580,7 +3580,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -3592,7 +3592,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -3604,7 +3604,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -3616,7 +3616,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -3628,7 +3628,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -3640,7 +3640,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -3652,7 +3652,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -3664,7 +3664,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -3676,7 +3676,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -3688,7 +3688,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -3700,7 +3700,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -3712,7 +3712,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -3724,7 +3724,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -3736,7 +3736,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -3748,7 +3748,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -3760,7 +3760,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -3784,7 +3784,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -3796,7 +3796,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -3808,7 +3808,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -3820,7 +3820,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -3832,7 +3832,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -3856,7 +3856,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -3868,7 +3868,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -3880,7 +3880,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -3892,7 +3892,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -3904,7 +3904,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -3916,7 +3916,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -3928,7 +3928,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -3940,7 +3940,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -3952,7 +3952,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -3964,7 +3964,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -3976,7 +3976,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -3988,7 +3988,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -4012,7 +4012,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -4024,7 +4024,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -4036,7 +4036,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -4048,7 +4048,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -4060,7 +4060,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>intellectual property rights</t>
+          <t>intellectual property</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">

</xml_diff>